<commit_message>
Fixed mistake, same game added twice.
</commit_message>
<xml_diff>
--- a/ChampMasteryData.xlsx
+++ b/ChampMasteryData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Final_Year\Summer 2016\Riot Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Final_Year\Summer 2016\Riot Project\ChampionMasteryPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Champion</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>B+</t>
+  </si>
+  <si>
+    <t>A-</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,6 +623,9 @@
       <c r="E7">
         <v>202</v>
       </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
@@ -631,31 +637,34 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="1">
+        <v>1.39375</v>
+      </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1">
-        <v>1.39375</v>
+      <c r="D9" s="2">
+        <v>0.97986111111111107</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>208</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more game data
</commit_message>
<xml_diff>
--- a/ChampMasteryData.xlsx
+++ b/ChampMasteryData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Champion</t>
   </si>
@@ -105,6 +105,66 @@
   </si>
   <si>
     <t>A-</t>
+  </si>
+  <si>
+    <t>Zac</t>
+  </si>
+  <si>
+    <t>Keno</t>
+  </si>
+  <si>
+    <t>Jhin</t>
+  </si>
+  <si>
+    <t>Blitz</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Maokai</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Greatest Forever</t>
+  </si>
+  <si>
+    <t>Lucian</t>
+  </si>
+  <si>
+    <t>Ezreal</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Seo</t>
+  </si>
+  <si>
+    <t>Riven</t>
+  </si>
+  <si>
+    <t>Kha'Zix</t>
+  </si>
+  <si>
+    <t>Draven</t>
+  </si>
+  <si>
+    <t>Hover</t>
+  </si>
+  <si>
+    <t>Sion</t>
+  </si>
+  <si>
+    <t>Party Bonus</t>
+  </si>
+  <si>
+    <t>Leona</t>
   </si>
 </sst>
 </file>
@@ -424,15 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
@@ -440,7 +500,7 @@
     <col min="8" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -471,8 +531,14 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -505,7 +571,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -538,7 +604,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -561,7 +627,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -584,7 +650,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -607,7 +673,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -633,7 +699,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -650,7 +716,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -665,6 +731,351 @@
       </c>
       <c r="J9">
         <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.5631944444444443</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.90069444444444446</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.90069444444444446</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.90069444444444446</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>337</v>
+      </c>
+      <c r="L15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.2395833333333333</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>220</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.2395833333333333</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>197</v>
+      </c>
+      <c r="K17">
+        <v>35</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.2395833333333333</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>197</v>
+      </c>
+      <c r="K18">
+        <v>37</v>
+      </c>
+      <c r="L18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.2395833333333333</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>197</v>
+      </c>
+      <c r="L19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.7388888888888889</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1458</v>
+      </c>
+      <c r="K20">
+        <v>278</v>
+      </c>
+      <c r="L20">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.7388888888888889</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1458</v>
+      </c>
+      <c r="K21">
+        <v>254</v>
+      </c>
+      <c r="L21">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.7388888888888889</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1458</v>
+      </c>
+      <c r="K22">
+        <v>283</v>
+      </c>
+      <c r="L22">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.7659722222222223</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1428</v>
+      </c>
+      <c r="K23">
+        <v>281</v>
+      </c>
+      <c r="L23">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.7659722222222223</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1428</v>
+      </c>
+      <c r="K24">
+        <v>287</v>
+      </c>
+      <c r="L24">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included graphs for wins and losses and fit a line.
</commit_message>
<xml_diff>
--- a/ChampMasteryData.xlsx
+++ b/ChampMasteryData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WinLoss Ratios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Champion</t>
   </si>
@@ -165,6 +166,18 @@
   </si>
   <si>
     <t>Leona</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -219,6 +232,1925 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Losses:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Points vs Time (mins)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35325502895706834"/>
+          <c:y val="2.724564009421199E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'WinLoss Ratios'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'WinLoss Ratios'!$D$3:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>309</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'WinLoss Ratios'!$E$3:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-773240592"/>
+        <c:axId val="-773241136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-773240592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773241136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-773241136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773240592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Wins: Points vs Time (mins)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'WinLoss Ratios'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'WinLoss Ratios'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1485</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>956</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'WinLoss Ratios'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-773249840"/>
+        <c:axId val="-773236784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-773249840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773236784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-773236784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-773249840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,10 +2416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +2672,9 @@
       <c r="B10" t="s">
         <v>27</v>
       </c>
+      <c r="D10" s="1">
+        <v>1.2319444444444445</v>
+      </c>
       <c r="F10" t="s">
         <v>25</v>
       </c>
@@ -1078,7 +3013,167 @@
         <v>54</v>
       </c>
     </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.0826388888888889</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>309</v>
+      </c>
+      <c r="K25">
+        <v>57</v>
+      </c>
+      <c r="L25">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1485</v>
+      </c>
+      <c r="C3">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>956</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>208</v>
+      </c>
+      <c r="E4">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1458</v>
+      </c>
+      <c r="C5">
+        <v>41.75</v>
+      </c>
+      <c r="D5">
+        <v>162</v>
+      </c>
+      <c r="E5">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1428</v>
+      </c>
+      <c r="C6">
+        <v>42.46</v>
+      </c>
+      <c r="D6">
+        <v>189</v>
+      </c>
+      <c r="E6">
+        <v>29.45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>229</v>
+      </c>
+      <c r="E7">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>167</v>
+      </c>
+      <c r="E8">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>337</v>
+      </c>
+      <c r="E9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>197</v>
+      </c>
+      <c r="E10">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>309</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more data, think we can use these models.
</commit_message>
<xml_diff>
--- a/ChampMasteryData.xlsx
+++ b/ChampMasteryData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="WinLoss Ratios" sheetId="2" r:id="rId2"/>
+    <sheet name="NameToID" sheetId="3" r:id="rId2"/>
+    <sheet name="WinLoss Ratios" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Champion</t>
   </si>
@@ -178,6 +179,12 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Iambbb</t>
+  </si>
+  <si>
+    <t>ryue</t>
   </si>
 </sst>
 </file>
@@ -268,25 +275,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Losses:</a:t>
+              <a:rPr lang="en-CA"/>
+              <a:t>Win</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Points vs Time (mins)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.35325502895706834"/>
-          <c:y val="2.724564009421199E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -325,17 +320,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'WinLoss Ratios'!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -370,76 +354,130 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.9827209098862645E-2"/>
+                  <c:y val="-0.1542341061533975"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'WinLoss Ratios'!$D$3:$D$11</c:f>
+              <c:f>'WinLoss Ratios'!$B$3:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>1485</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>208</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>162</c:v>
+                  <c:v>1458</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189</c:v>
+                  <c:v>1428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>229</c:v>
+                  <c:v>1065</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>167</c:v>
+                  <c:v>1260</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>337</c:v>
+                  <c:v>1230</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>197</c:v>
+                  <c:v>1230</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>309</c:v>
+                  <c:v>1598</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1237</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'WinLoss Ratios'!$E$3:$E$11</c:f>
+              <c:f>'WinLoss Ratios'!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>33.5</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.5</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.5</c:v>
+                  <c:v>41.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.45</c:v>
+                  <c:v>42.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.5</c:v>
+                  <c:v>30.783300000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.5</c:v>
+                  <c:v>33.266599999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>33.7333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.75</c:v>
+                  <c:v>33.566600000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>46.266599999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,11 +492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773240592"/>
-        <c:axId val="-773241136"/>
+        <c:axId val="1120965456"/>
+        <c:axId val="1120962192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773240592"/>
+        <c:axId val="1120965456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,12 +553,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773241136"/>
+        <c:crossAx val="1120962192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773241136"/>
+        <c:axId val="1120962192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773240592"/>
+        <c:crossAx val="1120965456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -660,8 +698,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Wins: Points vs Time (mins)</a:t>
+              <a:rPr lang="en-CA"/>
+              <a:t>Loss</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -705,17 +743,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'WinLoss Ratios'!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -754,42 +781,120 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'WinLoss Ratios'!$B$3:$B$6</c:f>
+              <c:f>'WinLoss Ratios'!$D$3:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1485</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>956</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1458</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1428</c:v>
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'WinLoss Ratios'!$C$3:$C$6</c:f>
+              <c:f>'WinLoss Ratios'!$E$3:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.75</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.46</c:v>
+                  <c:v>29.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.266599999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.7333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.716660000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33.566600000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46.266599999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.52</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,11 +909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773249840"/>
-        <c:axId val="-773236784"/>
+        <c:axId val="1121010000"/>
+        <c:axId val="1121009456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773249840"/>
+        <c:axId val="1121010000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,12 +970,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773236784"/>
+        <c:crossAx val="1121009456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773236784"/>
+        <c:axId val="1121009456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +1032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773249840"/>
+        <c:crossAx val="1121010000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2092,20 +2197,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2122,20 +2227,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2416,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3039,6 +3144,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.2826388888888889</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3046,15 +3168,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E11"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1">
+        <v>394891</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2">
+        <v>37074315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>47</v>
       </c>
@@ -3062,7 +3215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>49</v>
       </c>
@@ -3076,7 +3229,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1485</v>
       </c>
@@ -3090,7 +3243,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>956</v>
       </c>
@@ -3103,8 +3256,12 @@
       <c r="E4">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>AVERAGE(E3:E16)</f>
+        <v>34.303554285714277</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1458</v>
       </c>
@@ -3117,8 +3274,12 @@
       <c r="E5">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f>AVERAGE(C3:C10)</f>
+        <v>35.444974999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1428</v>
       </c>
@@ -3132,7 +3293,13 @@
         <v>29.45</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1065</v>
+      </c>
+      <c r="C7">
+        <v>30.783300000000001</v>
+      </c>
       <c r="D7">
         <v>229</v>
       </c>
@@ -3140,7 +3307,13 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1260</v>
+      </c>
+      <c r="C8">
+        <v>33.266599999999997</v>
+      </c>
       <c r="D8">
         <v>167</v>
       </c>
@@ -3148,7 +3321,13 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1230</v>
+      </c>
+      <c r="C9">
+        <v>33.7333</v>
+      </c>
       <c r="D9">
         <v>337</v>
       </c>
@@ -3156,7 +3335,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1230</v>
+      </c>
+      <c r="C10">
+        <v>33.566600000000001</v>
+      </c>
       <c r="D10">
         <v>197</v>
       </c>
@@ -3164,12 +3349,100 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1598</v>
+      </c>
+      <c r="C11">
+        <v>46.266599999999997</v>
+      </c>
       <c r="D11">
         <v>309</v>
       </c>
       <c r="E11">
         <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1237</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>219</v>
+      </c>
+      <c r="E12">
+        <v>33.266599999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>960</v>
+      </c>
+      <c r="C13">
+        <v>24.52</v>
+      </c>
+      <c r="D13">
+        <v>207</v>
+      </c>
+      <c r="E13">
+        <v>33.7333</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1466</v>
+      </c>
+      <c r="C14">
+        <v>42.5</v>
+      </c>
+      <c r="D14">
+        <v>151</v>
+      </c>
+      <c r="E14">
+        <v>20.716660000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>210</v>
+      </c>
+      <c r="E15">
+        <v>33.566600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>296</v>
+      </c>
+      <c r="E16">
+        <v>46.266599999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>203</v>
+      </c>
+      <c r="E17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>155</v>
+      </c>
+      <c r="E18">
+        <v>24.52</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>160</v>
+      </c>
+      <c r="E19">
+        <v>25.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still working on champ.
</commit_message>
<xml_diff>
--- a/ChampMasteryData.xlsx
+++ b/ChampMasteryData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4125" windowHeight="6150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,8 +358,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.9827209098862645E-2"/>
-                  <c:y val="-0.1542341061533975"/>
+                  <c:x val="-0.13316054243219597"/>
+                  <c:y val="3.1733012540099154E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -777,7 +777,43 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10709711286089239"/>
+                  <c:y val="6.6112933799941667E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -2523,7 +2559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>

</xml_diff>